<commit_message>
fix modelsettings iniwlvl empty cols
</commit_message>
<xml_diff>
--- a/hhnk_threedi_tools/resources/model_settings.xlsx
+++ b/hhnk_threedi_tools/resources/model_settings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp.hhnk.nl\data\Hydrologen_data\Data\github\jkaptein\hhnk-threedi-tools\hhnk_threedi_tools\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp.hhnk.nl\data\hydrologen_data\Data\github\wvangerwen\hhnk-threedi-tools\hhnk_threedi_tools\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40E1BF3-DCC8-4AAD-B59D-959375E497C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AD63E2-44FC-4BDB-ABCB-C8A3421B50C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -67,84 +67,6 @@
     <t>infiltration_surface_option</t>
   </si>
   <si>
-    <t>Unnamed: 18</t>
-  </si>
-  <si>
-    <t>Unnamed: 19</t>
-  </si>
-  <si>
-    <t>Unnamed: 20</t>
-  </si>
-  <si>
-    <t>Unnamed: 21</t>
-  </si>
-  <si>
-    <t>Unnamed: 22</t>
-  </si>
-  <si>
-    <t>Unnamed: 23</t>
-  </si>
-  <si>
-    <t>Unnamed: 24</t>
-  </si>
-  <si>
-    <t>Unnamed: 25</t>
-  </si>
-  <si>
-    <t>Unnamed: 26</t>
-  </si>
-  <si>
-    <t>Unnamed: 27</t>
-  </si>
-  <si>
-    <t>Unnamed: 28</t>
-  </si>
-  <si>
-    <t>Unnamed: 29</t>
-  </si>
-  <si>
-    <t>Unnamed: 30</t>
-  </si>
-  <si>
-    <t>Unnamed: 31</t>
-  </si>
-  <si>
-    <t>Unnamed: 32</t>
-  </si>
-  <si>
-    <t>Unnamed: 33</t>
-  </si>
-  <si>
-    <t>Unnamed: 34</t>
-  </si>
-  <si>
-    <t>Unnamed: 35</t>
-  </si>
-  <si>
-    <t>Unnamed: 36</t>
-  </si>
-  <si>
-    <t>Unnamed: 37</t>
-  </si>
-  <si>
-    <t>Unnamed: 38</t>
-  </si>
-  <si>
-    <t>Unnamed: 39</t>
-  </si>
-  <si>
-    <t>Unnamed: 40</t>
-  </si>
-  <si>
-    <t>Unnamed: 41</t>
-  </si>
-  <si>
-    <t>Unnamed: 42</t>
-  </si>
-  <si>
-    <t>Unnamed: 43</t>
-  </si>
-  <si>
     <t>glg</t>
   </si>
   <si>
@@ -212,6 +134,9 @@
   </si>
   <si>
     <t>rasters/storage_ghg_callantsoog.tif</t>
+  </si>
+  <si>
+    <t>water_level_ini_type</t>
   </si>
 </sst>
 </file>
@@ -582,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,19 +520,19 @@
     <col min="4" max="4" width="44.85546875" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.140625" customWidth="1"/>
-    <col min="7" max="7" width="36" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" customWidth="1"/>
+    <col min="7" max="9" width="36" customWidth="1"/>
+    <col min="10" max="10" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -622,355 +547,280 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="T1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG1" s="1" t="s">
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>40</v>
+      <c r="K2">
+        <v>900</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2">
-        <v>900</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>4</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3">
+        <v>30</v>
+      </c>
+      <c r="K3">
         <v>300</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <v>4</v>
       </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
+      <c r="N3">
         <v>1</v>
       </c>
       <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="T3">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4">
         <v>300</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>4</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5">
         <v>300</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
         <v>4</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
       <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
         <v>2</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6">
         <v>300</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>4</v>
       </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
       <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
         <v>3</v>
       </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Model splitter fixes (#65)
* Update model_splitter.py

* Update model_splitter.py

* synced model_Settings

* sync environments

* Update model_settings.xlsx

* update version

* false cont  and add foldertest on threediresults

---------

Co-authored-by: Wietse van Gerwen <41104904+wvangerwen@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/hhnk_threedi_tools/resources/model_settings.xlsx
+++ b/hhnk_threedi_tools/resources/model_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp.hhnk.nl\data\hydrologen_data\Data\github\wvangerwen\hhnk-threedi-tools\hhnk_threedi_tools\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\hhnk-threedi-tools\hhnk_threedi_tools\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AD63E2-44FC-4BDB-ABCB-C8A3421B50C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4576C8AA-2559-4A7F-8B12-E8FE460D09E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>1d2d_ghg</t>
-  </si>
-  <si>
-    <t>grid_space</t>
   </si>
   <si>
     <t>initial_waterlevel_file</t>
@@ -206,8 +203,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{229E95DB-BF8D-415B-AF0D-AA2F4605D28A}"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -507,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +521,7 @@
     <col min="10" max="10" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,10 +544,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
@@ -582,22 +579,19 @@
       <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2">
         <v>900</v>
@@ -606,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -614,25 +608,22 @@
       <c r="Q2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K3">
         <v>300</v>
@@ -641,7 +632,7 @@
         <v>1</v>
       </c>
       <c r="M3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -652,31 +643,28 @@
       <c r="Q3">
         <v>0</v>
       </c>
-      <c r="T3">
-        <v>12</v>
-      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
         <v>32</v>
-      </c>
-      <c r="G4" t="s">
-        <v>33</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
@@ -688,7 +676,7 @@
         <v>1</v>
       </c>
       <c r="M4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -708,31 +696,28 @@
       <c r="S4">
         <v>0</v>
       </c>
-      <c r="T4">
-        <v>12</v>
-      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" t="s">
         <v>16</v>
@@ -744,7 +729,7 @@
         <v>1</v>
       </c>
       <c r="M5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -764,31 +749,28 @@
       <c r="S5">
         <v>0</v>
       </c>
-      <c r="T5">
-        <v>12</v>
-      </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
         <v>17</v>
@@ -800,7 +782,7 @@
         <v>1</v>
       </c>
       <c r="M6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -819,9 +801,6 @@
       </c>
       <c r="S6">
         <v>0</v>
-      </c>
-      <c r="T6">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>